<commit_message>
fix for email and service related issues for downloading documents.
</commit_message>
<xml_diff>
--- a/src/main/resources/json/AppConfiguration.xlsx
+++ b/src/main/resources/json/AppConfiguration.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20361"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{249D2874-0E6C-4CC8-AA91-5E01AA5EAFA4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1483F127-665C-414D-B580-79D98AFF2904}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="117">
   <si>
     <t>planId</t>
   </si>
@@ -298,6 +298,84 @@
   </si>
   <si>
     <t>Employee2</t>
+  </si>
+  <si>
+    <t>[</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "planId": "101",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "validityDays": "365",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "planName": "FREE",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "planBuyPrice": "0",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "planActualPrice": "0",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "planCurrency": "INR",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "planStatus": "ACTIVE",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "countryId": "IND",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "planType": "APP_ACTIVATE",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "planDesc": "All Free app functions are available for the user. All App functions can be used offline on device. Ad's will be available when online. Following are app main utils: \\n* Manage Asset &amp; Family. \\n* Manage Portfolio's \\n* Notes \\n* Plan List \\n* Calendar \\n* Self Tracker "</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "planId": "102",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "planName": "PRIME-FAMILY",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "planBuyPrice": "299",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "planActualPrice": "299",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "planId": "103",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "validityDays": "1111",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "planName": "PRICE-INFLUENCER",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "planBuyPrice": "999",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "planActualPrice": "999",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "planDesc": "All Free app functions are available for the user. All App functions can be used offline on device. Ad's will be available when online. Following are app main utils: \\n* Manage Asset &amp; Family. \\n* Manage Portfolio's \\n* Notes \\n* Plan List \\n* Calendar \\n* Self Tracker"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    }</t>
+  </si>
+  <si>
+    <t>]</t>
+  </si>
+  <si>
+    <t>https://tableconvert.com/excel-to-json</t>
   </si>
 </sst>
 </file>
@@ -668,10 +746,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -816,6 +894,201 @@
         <v>16</v>
       </c>
     </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="B12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="B13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="B14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="B15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="B16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2">
+      <c r="B26" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2">
+      <c r="B27" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2">
+      <c r="B28" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2">
+      <c r="B29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2">
+      <c r="B30" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2">
+      <c r="B31" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2">
+      <c r="B32" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2">
+      <c r="B37" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2">
+      <c r="B38" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2">
+      <c r="B39" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2">
+      <c r="B40" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2">
+      <c r="B41" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2">
+      <c r="B42" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2">
+      <c r="B43" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2">
+      <c r="B44" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2">
+      <c r="B45" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2">
+      <c r="B46" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2">
+      <c r="B47" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2">
+      <c r="B48" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2">
+      <c r="B49" t="s">
+        <v>115</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -827,10 +1100,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B96CFD03-D994-4F25-92D3-FD2B55886A52}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -963,6 +1236,11 @@
         <v>36</v>
       </c>
     </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>116</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -970,10 +1248,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA79140B-0174-4511-B8BB-44A0EBFF1A39}">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1400,6 +1678,11 @@
         <v>2</v>
       </c>
     </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>116</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1407,38 +1690,60 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3858027-154E-4941-8A4B-7600298E9887}">
-  <dimension ref="A1"/>
+  <dimension ref="A17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
+  <sheetData>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>116</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{581468F8-1DD1-451F-9D78-65444399546B}">
-  <dimension ref="A1"/>
+  <dimension ref="A18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
+  <sheetData>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1D3892C-303C-4DF9-9075-0B8E88FB5B24}">
-  <dimension ref="A1"/>
+  <dimension ref="A16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
+  <sheetData>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>